<commit_message>
fixed groups spreadsheet path in setup service. updated bashrc with dropdb and createdb commands. removed few extra rows and columns in template files
</commit_message>
<xml_diff>
--- a/app-conf/data/datarep/species/templates/Classifications.xlsx
+++ b/app-conf/data/datarep/species/templates/Classifications.xlsx
@@ -37,31 +37,31 @@
     <t>Hierarchy contributed by the species page author</t>
   </si>
   <si>
+    <t>GBIF Taxonomy Hierarchy</t>
+  </si>
+  <si>
+    <t>&lt;a target='_blank' href='http://data.gbif.org/datasets/resource/1'&gt;Accessed through GBIF data portal, GBIF Backbone Taxonomy&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>IUCN Taxonomy Hierarchy (2010)</t>
+  </si>
+  <si>
+    <t>&lt;a target='_blank'  href='www.iucnredlist.org'&gt;IUCN 2011. IUCN Red List of Threatened Species. Version 2011.2. Exported on 12 January 2012&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>FishBase Taxonomy Hierarchy</t>
+  </si>
+  <si>
+    <t>Froese, R. and D. Pauly. Editors. 2011.FishBase.World Wide Web electronic publication.&lt;a href='http://www.fishbase.org/' target='_blank' &gt;www.fishbase.org, version (10/2011).&lt;/a&gt;</t>
+  </si>
+  <si>
     <t>Eflora Taxonomy Hierarchy</t>
   </si>
   <si>
-    <t>GBIF Taxonomy Hierarchy</t>
-  </si>
-  <si>
-    <t>&lt;a target='_blank' href='http://data.gbif.org/datasets/resource/1'&gt;Accessed through GBIF data portal, GBIF Backbone Taxonomy&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>ITIS Taxonomy Hierarchy</t>
   </si>
   <si>
-    <t>IUCN Taxonomy Hierarchy (2010)</t>
-  </si>
-  <si>
-    <t>&lt;a target='_blank'  href='www.iucnredlist.org'&gt;IUCN 2011. IUCN Red List of Threatened Species. Version 2011.2. Exported on 12 January 2012&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Wikipedia Taxonomy Hierarchy</t>
-  </si>
-  <si>
-    <t>FishBase Taxonomy Hierarchy</t>
-  </si>
-  <si>
-    <t>Froese, R. and D. Pauly. Editors. 2011.FishBase.World Wide Web electronic publication.&lt;a href='http://www.fishbase.org/' target='_blank' &gt;www.fishbase.org, version (10/2011).&lt;/a&gt;</t>
   </si>
   <si>
     <t>Sibley and Monroe Taxonomy Hierarchy (1996)</t>
@@ -98,6 +98,7 @@
   <fonts count="6">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="11"/>
@@ -119,12 +120,14 @@
     </font>
     <font>
       <name val="Arial Narrow"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000000"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial Narrow"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00000000"/>
@@ -204,22 +207,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B7" activeCellId="0" pane="topLeft" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.8862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="67.8941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.1764705882353"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.6666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.0117647058823"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="68.1725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.3372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.8313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.89803921568628"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -229,7 +232,7 @@
       <c r="C1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -239,7 +242,7 @@
       <c r="C2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -247,82 +250,35 @@
         <v>5</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="0"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D4" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
-      <c r="B7" s="4"/>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
-      <c r="B8" s="4"/>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
-      <c r="B9" s="4"/>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
-      <c r="B13" s="4"/>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -345,16 +301,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.89803921568628"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="4">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="6">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="8">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="9">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="10">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="11">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
@@ -372,12 +385,12 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89803921568628"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>